<commit_message>
Review and minor changes for mappings of Zibs SkinDisorder, AbilityToPerformNursingActivites and DevelopmentChild
</commit_message>
<xml_diff>
--- a/Mappings/DevelopmentChild - STU3.xlsx
+++ b/Mappings/DevelopmentChild - STU3.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edelman\Nictiz-STU3-Zib2017\Mappings\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26DF402-D565-4D88-BDA2-A128B35D08C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13995" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13995" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -20,7 +26,7 @@
     <sheet name="ToiletTrainednessUrineCodelist" sheetId="10" r:id="rId11"/>
     <sheet name="Terms of Use" sheetId="11" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="0" iterate="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -783,9 +789,6 @@
     <t>Valueset reference</t>
   </si>
   <si>
-    <t>Observation</t>
-  </si>
-  <si>
     <t>.effectiveDatetime</t>
   </si>
   <si>
@@ -817,13 +820,16 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>nl-core-observation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -962,7 +968,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1006,9 +1012,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1018,6 +1021,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1029,6 +1038,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1099,7 +1111,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1142,7 +1154,13 @@
     <xdr:ext cx="2856900" cy="618995"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPr id="1025" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1177,7 +1195,13 @@
     <xdr:ext cx="1428750" cy="504825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1026" name="Picture 2"/>
+        <xdr:cNvPr id="1026" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1212,7 +1236,13 @@
     <xdr:ext cx="7334250" cy="6029325"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPr id="1025" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1264,11 +1294,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3073"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000010C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1276,6 +1309,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1305,11 +1361,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3074"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000020C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1317,6 +1376,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1346,11 +1428,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3075"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000030C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1358,6 +1443,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1387,11 +1495,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3076"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000040C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1399,6 +1510,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1428,11 +1562,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3077"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000050C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1440,6 +1577,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1469,11 +1629,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3078"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000060C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1481,6 +1644,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1510,11 +1696,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3079"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000070C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1522,6 +1711,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1551,11 +1763,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3080"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000080C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1563,6 +1778,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1592,11 +1830,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3081"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000090C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1604,6 +1845,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1633,11 +1897,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3082"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A0C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1645,6 +1912,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1674,11 +1964,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3083"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B0C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1686,6 +1979,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1715,11 +2031,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3084"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C0C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1727,6 +2046,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1756,11 +2098,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3085"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D0C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1768,6 +2113,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1797,11 +2165,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3086"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E0C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1809,6 +2180,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1838,11 +2232,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3087"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000F0C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1850,6 +2247,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1879,11 +2299,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3088"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000100C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1891,6 +2314,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1920,11 +2366,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3089"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000110C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1932,6 +2381,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1961,11 +2433,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3090"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000120C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1973,6 +2448,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1992,8 +2490,8 @@
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2002,11 +2500,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3091"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000130C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2014,6 +2515,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2033,8 +2557,8 @@
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2043,11 +2567,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3092"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000140C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2055,6 +2582,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2074,8 +2624,8 @@
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2084,11 +2634,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3093"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000150C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2096,6 +2649,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2115,8 +2691,8 @@
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2125,11 +2701,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3094"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000160C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2137,6 +2716,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2156,8 +2758,8 @@
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2166,11 +2768,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3095"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000170C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2178,6 +2783,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2197,8 +2825,8 @@
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2207,11 +2835,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3096"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000180C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2219,6 +2850,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2272,7 +2926,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2305,9 +2959,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2340,6 +3011,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2515,18 +3203,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2534,7 +3222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2542,7 +3230,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2550,7 +3238,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2558,7 +3246,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -2566,7 +3254,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -2574,7 +3262,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -2582,7 +3270,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
@@ -2590,7 +3278,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
@@ -2598,7 +3286,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
@@ -2606,7 +3294,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="38.25">
+    <row r="12" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>54</v>
       </c>
@@ -2614,7 +3302,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="63.75">
+    <row r="13" spans="2:3" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>56</v>
       </c>
@@ -2622,7 +3310,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="38.25">
+    <row r="14" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>58</v>
       </c>
@@ -2630,7 +3318,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="51">
+    <row r="15" spans="2:3" ht="51" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>132</v>
       </c>
@@ -2640,7 +3328,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1"/>
+    <hyperlink ref="C11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2651,12 +3339,12 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="C3:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -2665,18 +3353,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="15" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="3:7">
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
         <v>135</v>
       </c>
@@ -2693,7 +3381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="25.5">
+    <row r="5" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>205</v>
       </c>
@@ -2710,7 +3398,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="25.5">
+    <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>208</v>
       </c>
@@ -2727,7 +3415,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="25.5">
+    <row r="7" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>211</v>
       </c>
@@ -2757,12 +3445,12 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="C3:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -2771,18 +3459,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="15" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="3:7">
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
         <v>135</v>
       </c>
@@ -2799,7 +3487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="25.5">
+    <row r="5" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>215</v>
       </c>
@@ -2816,7 +3504,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="25.5">
+    <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>217</v>
       </c>
@@ -2833,7 +3521,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="25.5">
+    <row r="7" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>220</v>
       </c>
@@ -2850,7 +3538,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="25.5">
+    <row r="8" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C8" s="2" t="s">
         <v>222</v>
       </c>
@@ -2880,42 +3568,42 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="B2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="150" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="140.25">
+    <row r="3" spans="2:2" ht="140.25" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="25.5">
+    <row r="5" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="38.25">
+    <row r="7" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>229</v>
       </c>
@@ -2926,24 +3614,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
-      <c r="B2" s="15" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="15"/>
-    </row>
-    <row r="3" spans="2:3">
+      <c r="C2" s="21"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
@@ -2951,7 +3639,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
@@ -2959,7 +3647,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
@@ -2967,7 +3655,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
@@ -2975,7 +3663,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -2983,7 +3671,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
@@ -2991,13 +3679,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
@@ -3005,25 +3693,25 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>36</v>
       </c>
@@ -3031,7 +3719,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>38</v>
       </c>
@@ -3039,7 +3727,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>40</v>
       </c>
@@ -3047,7 +3735,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>41</v>
       </c>
@@ -3055,7 +3743,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>42</v>
       </c>
@@ -3063,7 +3751,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>44</v>
       </c>
@@ -3071,7 +3759,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>45</v>
       </c>
@@ -3079,7 +3767,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>46</v>
       </c>
@@ -3087,7 +3775,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
@@ -3095,7 +3783,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>49</v>
       </c>
@@ -3103,7 +3791,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>51</v>
       </c>
@@ -3111,7 +3799,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>52</v>
       </c>
@@ -3131,14 +3819,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
     </row>
   </sheetData>
@@ -3148,124 +3836,124 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="51.140625" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="27.85546875" customWidth="1"/>
     <col min="4" max="4" width="79.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="78.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="H1" s="16"/>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="17" t="s">
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="17" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="17" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="17" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="17" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="17" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="17" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="17" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="17" t="s">
+    <row r="10" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
         <v>242</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="22" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="19"/>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1"/>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -3683,8 +4371,8 @@
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3705,8 +4393,8 @@
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3727,8 +4415,8 @@
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3749,8 +4437,8 @@
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3771,8 +4459,8 @@
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3793,8 +4481,8 @@
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3808,14 +4496,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:T12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="6" width="2" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
@@ -3829,7 +4517,7 @@
     <col min="20" max="20" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>54</v>
       </c>
@@ -3872,13 +4560,13 @@
         <v>250</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="2:20" ht="38.25">
+    <row r="3" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
         <v>69</v>
       </c>
@@ -3906,14 +4594,14 @@
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
     </row>
-    <row r="4" spans="2:20" ht="25.5">
+    <row r="4" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B4" s="11"/>
       <c r="C4" s="12" t="s">
         <v>75</v>
@@ -3943,16 +4631,16 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="Q4" s="20" t="s">
-        <v>261</v>
+        <v>251</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>260</v>
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="2:20" ht="38.25">
+    <row r="5" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B5" s="11"/>
       <c r="C5" s="12" t="s">
         <v>82</v>
@@ -3985,19 +4673,19 @@
       <c r="O5" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="P5" s="20" t="s">
+      <c r="P5" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q5" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="Q5" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="R5" s="20" t="s">
+      <c r="R5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="S5" s="20"/>
+      <c r="S5" s="19"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="2:20" ht="38.25">
+    <row r="6" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
         <v>90</v>
@@ -4030,21 +4718,21 @@
       <c r="O6" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="P6" s="20" t="s">
-        <v>259</v>
-      </c>
-      <c r="Q6" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="R6" s="20" t="s">
+      <c r="P6" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q6" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="R6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="S6" s="20"/>
+      <c r="S6" s="19"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="2:20" ht="25.5">
+    <row r="7" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B7" s="11"/>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>96</v>
       </c>
       <c r="D7" s="12"/>
@@ -4073,21 +4761,21 @@
         <v>101</v>
       </c>
       <c r="O7" s="2"/>
-      <c r="P7" s="20" t="s">
-        <v>258</v>
-      </c>
-      <c r="Q7" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="R7" s="20" t="s">
+      <c r="P7" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q7" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="R7" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="S7" s="20"/>
+      <c r="S7" s="19"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="2:20" ht="38.25">
+    <row r="8" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B8" s="11"/>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="20" t="s">
         <v>102</v>
       </c>
       <c r="D8" s="12"/>
@@ -4118,21 +4806,21 @@
       <c r="O8" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="P8" s="20" t="s">
-        <v>257</v>
-      </c>
-      <c r="Q8" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="R8" s="20" t="s">
+      <c r="P8" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q8" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="R8" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="S8" s="20"/>
+      <c r="S8" s="19"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="2:20" ht="38.25">
+    <row r="9" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B9" s="11"/>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="20" t="s">
         <v>108</v>
       </c>
       <c r="D9" s="12"/>
@@ -4163,21 +4851,21 @@
       <c r="O9" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="P9" s="20" t="s">
-        <v>256</v>
-      </c>
-      <c r="Q9" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="R9" s="20" t="s">
+      <c r="P9" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q9" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="R9" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="S9" s="20"/>
+      <c r="S9" s="19"/>
       <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="2:20" ht="38.25">
+    <row r="10" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B10" s="11"/>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="20" t="s">
         <v>114</v>
       </c>
       <c r="D10" s="12"/>
@@ -4208,21 +4896,21 @@
       <c r="O10" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="P10" s="20" t="s">
-        <v>255</v>
-      </c>
-      <c r="Q10" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="R10" s="20" t="s">
+      <c r="P10" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q10" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="R10" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="S10" s="20"/>
+      <c r="S10" s="19"/>
       <c r="T10" s="2"/>
     </row>
-    <row r="11" spans="2:20" ht="38.25">
+    <row r="11" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B11" s="11"/>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="20" t="s">
         <v>120</v>
       </c>
       <c r="D11" s="12"/>
@@ -4253,19 +4941,19 @@
       <c r="O11" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="P11" s="20" t="s">
-        <v>254</v>
-      </c>
-      <c r="Q11" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="R11" s="20" t="s">
+      <c r="P11" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q11" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="R11" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="S11" s="20"/>
+      <c r="S11" s="19"/>
       <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="2:20" ht="25.5">
+    <row r="12" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B12" s="11"/>
       <c r="C12" s="12" t="s">
         <v>126</v>
@@ -4296,11 +4984,11 @@
         <v>131</v>
       </c>
       <c r="O12" s="2"/>
-      <c r="P12" s="20" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q12" s="20" t="s">
-        <v>261</v>
+      <c r="P12" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q12" s="19" t="s">
+        <v>260</v>
       </c>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
@@ -4308,12 +4996,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O5" location="ToiletTrainednessUrineCodelist!A1" display="ToiletTrainednessUrineCodelist"/>
-    <hyperlink ref="O6" location="ToiletTrainednessFecesCodelist!A1" display="ToiletTrainednessFecesCodelist"/>
-    <hyperlink ref="O8" location="DevelopmentLocomotionCodelist!A1" display="DevelopmentLocomotionCodelist"/>
-    <hyperlink ref="O9" location="DevelopmentSocialCodelist!A1" display="DevelopmentSocialCodelist"/>
-    <hyperlink ref="O10" location="DevelopmentLinguisticsCodelist!A1" display="DevelopmentLinguisticsCodelist"/>
-    <hyperlink ref="O11" location="DevelopmentCognitionCodelist!A1" display="DevelopmentCognitionCodelist"/>
+    <hyperlink ref="O5" location="ToiletTrainednessUrineCodelist!A1" display="ToiletTrainednessUrineCodelist" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="O6" location="ToiletTrainednessFecesCodelist!A1" display="ToiletTrainednessFecesCodelist" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="O8" location="DevelopmentLocomotionCodelist!A1" display="DevelopmentLocomotionCodelist" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="O9" location="DevelopmentSocialCodelist!A1" display="DevelopmentSocialCodelist" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="O10" location="DevelopmentLinguisticsCodelist!A1" display="DevelopmentLinguisticsCodelist" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="O11" location="DevelopmentCognitionCodelist!A1" display="DevelopmentCognitionCodelist" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4324,12 +5012,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="C3:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -4338,18 +5026,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="15" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="3:7">
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
         <v>135</v>
       </c>
@@ -4366,7 +5054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>139</v>
       </c>
@@ -4383,7 +5071,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="3:7">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>144</v>
       </c>
@@ -4400,7 +5088,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="25.5">
+    <row r="7" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>147</v>
       </c>
@@ -4417,7 +5105,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="25.5">
+    <row r="8" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C8" s="2" t="s">
         <v>150</v>
       </c>
@@ -4434,7 +5122,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="3:7" ht="25.5">
+    <row r="9" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="s">
         <v>153</v>
       </c>
@@ -4464,12 +5152,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="C3:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -4478,18 +5166,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="15" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="3:7">
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
         <v>135</v>
       </c>
@@ -4506,7 +5194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>157</v>
       </c>
@@ -4523,7 +5211,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="25.5">
+    <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>160</v>
       </c>
@@ -4540,7 +5228,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="25.5">
+    <row r="7" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>163</v>
       </c>
@@ -4557,7 +5245,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="25.5">
+    <row r="8" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C8" s="2" t="s">
         <v>166</v>
       </c>
@@ -4574,7 +5262,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="3:7" ht="25.5">
+    <row r="9" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="s">
         <v>169</v>
       </c>
@@ -4604,12 +5292,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="C3:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -4618,18 +5306,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="15" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="3:7">
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
         <v>135</v>
       </c>
@@ -4646,7 +5334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>173</v>
       </c>
@@ -4663,7 +5351,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="3:7">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>176</v>
       </c>
@@ -4680,7 +5368,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="3:7">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>179</v>
       </c>
@@ -4697,7 +5385,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="25.5">
+    <row r="8" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C8" s="2" t="s">
         <v>182</v>
       </c>
@@ -4714,7 +5402,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="3:7">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="s">
         <v>185</v>
       </c>
@@ -4744,12 +5432,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="C3:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -4758,18 +5446,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="15" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="3:7">
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
         <v>135</v>
       </c>
@@ -4786,7 +5474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="25.5">
+    <row r="5" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>189</v>
       </c>
@@ -4803,7 +5491,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="25.5">
+    <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>192</v>
       </c>
@@ -4820,7 +5508,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="25.5">
+    <row r="7" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>195</v>
       </c>
@@ -4837,7 +5525,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="25.5">
+    <row r="8" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C8" s="2" t="s">
         <v>198</v>
       </c>
@@ -4854,7 +5542,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="3:7" ht="25.5">
+    <row r="9" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="s">
         <v>201</v>
       </c>

</xml_diff>

<commit_message>
add: profile, example, valuesets for zib-DevelopmentChild
</commit_message>
<xml_diff>
--- a/Mappings/DevelopmentChild - STU3.xlsx
+++ b/Mappings/DevelopmentChild - STU3.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edelman\Nictiz-STU3-Zib2017\Mappings\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26DF402-D565-4D88-BDA2-A128B35D08C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13995" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13995" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -807,9 +801,6 @@
     <t>.component.developmentLocomotion.valueCodeableConcept</t>
   </si>
   <si>
-    <t>.component.ageFirstMenstruation.valueCodeableConcept</t>
-  </si>
-  <si>
     <t>.component.toiletTrainednessFeces.valueCodeableConcept</t>
   </si>
   <si>
@@ -823,13 +814,16 @@
   </si>
   <si>
     <t>nl-core-observation</t>
+  </si>
+  <si>
+    <t>.component.ageFirstMenstruation.valueDateTime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -1022,11 +1016,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1157,7 +1151,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1198,7 +1192,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1239,7 +1233,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1294,14 +1288,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3073"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000010C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1309,29 +1300,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1361,14 +1329,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3074"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000020C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1376,29 +1341,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1428,14 +1370,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3075"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000030C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1443,29 +1382,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1495,14 +1411,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3076"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000040C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1510,29 +1423,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1562,14 +1452,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3077"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000050C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1577,29 +1464,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1629,14 +1493,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3078"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000060C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1644,29 +1505,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1696,14 +1534,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3079"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000070C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1711,29 +1546,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1763,14 +1575,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3080"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000080C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1778,29 +1587,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1830,14 +1616,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3081"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000090C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1845,29 +1628,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1897,14 +1657,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3082"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1912,29 +1669,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1964,14 +1698,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3083"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1979,29 +1710,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2031,14 +1739,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3084"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2046,29 +1751,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2098,14 +1780,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3085"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2113,29 +1792,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2165,14 +1821,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3086"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2180,29 +1833,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2232,14 +1862,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3087"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000F0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2247,29 +1874,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2299,14 +1903,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3088"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000100C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2314,29 +1915,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2366,14 +1944,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3089"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000110C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2381,29 +1956,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2433,14 +1985,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3090"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000120C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2448,29 +1997,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2500,14 +2026,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3091"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000130C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2515,29 +2038,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2567,14 +2067,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3092"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000140C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2582,29 +2079,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2634,14 +2108,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3093"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000150C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2649,29 +2120,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2701,14 +2149,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3094"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000160C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2716,29 +2161,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2768,14 +2190,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3095"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000170C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2783,29 +2202,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2835,14 +2231,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3096"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000180C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2850,29 +2243,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2926,7 +2296,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2959,26 +2329,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3011,23 +2364,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3203,18 +2539,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3222,7 +2558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -3230,7 +2566,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -3238,7 +2574,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -3246,7 +2582,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -3254,7 +2590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -3262,7 +2598,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -3270,7 +2606,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3">
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
@@ -3278,7 +2614,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3">
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
@@ -3286,7 +2622,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3">
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
@@ -3294,7 +2630,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3" ht="38.25">
       <c r="B12" s="2" t="s">
         <v>54</v>
       </c>
@@ -3302,7 +2638,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3" ht="63.75">
       <c r="B13" s="2" t="s">
         <v>56</v>
       </c>
@@ -3310,7 +2646,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3" ht="38.25">
       <c r="B14" s="2" t="s">
         <v>58</v>
       </c>
@@ -3318,7 +2654,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:3" ht="51">
       <c r="B15" s="2" t="s">
         <v>132</v>
       </c>
@@ -3328,7 +2664,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3339,12 +2675,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:G3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -3353,18 +2691,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="21" t="s">
+    <row r="3" spans="3:7">
+      <c r="C3" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="3:7">
       <c r="C4" s="14" t="s">
         <v>135</v>
       </c>
@@ -3381,7 +2719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:7" ht="25.5">
       <c r="C5" s="2" t="s">
         <v>205</v>
       </c>
@@ -3398,7 +2736,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:7" ht="25.5">
       <c r="C6" s="2" t="s">
         <v>208</v>
       </c>
@@ -3415,7 +2753,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:7" ht="25.5">
       <c r="C7" s="2" t="s">
         <v>211</v>
       </c>
@@ -3445,12 +2783,12 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -3459,18 +2797,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="21" t="s">
+    <row r="3" spans="3:7">
+      <c r="C3" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="3:7">
       <c r="C4" s="14" t="s">
         <v>135</v>
       </c>
@@ -3487,7 +2825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:7" ht="25.5">
       <c r="C5" s="2" t="s">
         <v>215</v>
       </c>
@@ -3504,7 +2842,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:7" ht="25.5">
       <c r="C6" s="2" t="s">
         <v>217</v>
       </c>
@@ -3521,7 +2859,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:7" ht="25.5">
       <c r="C7" s="2" t="s">
         <v>220</v>
       </c>
@@ -3538,7 +2876,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:7" ht="25.5">
       <c r="C8" s="2" t="s">
         <v>222</v>
       </c>
@@ -3568,42 +2906,42 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="150" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:2">
       <c r="B2" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:2" ht="140.25">
       <c r="B3" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:2">
       <c r="B4" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:2" ht="25.5">
       <c r="B5" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:2">
       <c r="B6" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:2" ht="38.25">
       <c r="B7" s="2" t="s">
         <v>229</v>
       </c>
@@ -3614,24 +2952,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="21" t="s">
+    <row r="2" spans="2:3">
+      <c r="B2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="21"/>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C2" s="22"/>
+    </row>
+    <row r="3" spans="2:3">
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
@@ -3639,7 +2977,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3">
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
@@ -3647,7 +2985,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3">
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
@@ -3655,7 +2993,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3">
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
@@ -3663,7 +3001,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -3671,7 +3009,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3">
       <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
@@ -3679,13 +3017,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3">
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3">
       <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
@@ -3693,25 +3031,25 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3">
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3">
       <c r="B13" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3">
       <c r="B14" s="2" t="s">
         <v>36</v>
       </c>
@@ -3719,7 +3057,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:3">
       <c r="B15" s="2" t="s">
         <v>38</v>
       </c>
@@ -3727,7 +3065,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:3">
       <c r="B16" s="2" t="s">
         <v>40</v>
       </c>
@@ -3735,7 +3073,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3">
       <c r="B17" s="2" t="s">
         <v>41</v>
       </c>
@@ -3743,7 +3081,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3">
       <c r="B18" s="2" t="s">
         <v>42</v>
       </c>
@@ -3751,7 +3089,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3">
       <c r="B19" s="2" t="s">
         <v>44</v>
       </c>
@@ -3759,7 +3097,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3">
       <c r="B20" s="2" t="s">
         <v>45</v>
       </c>
@@ -3767,7 +3105,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3">
       <c r="B21" s="2" t="s">
         <v>46</v>
       </c>
@@ -3775,7 +3113,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3">
       <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
@@ -3783,7 +3121,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3">
       <c r="B23" s="2" t="s">
         <v>49</v>
       </c>
@@ -3791,7 +3129,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3">
       <c r="B24" s="2" t="s">
         <v>51</v>
       </c>
@@ -3799,7 +3137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3">
       <c r="B25" s="2" t="s">
         <v>52</v>
       </c>
@@ -3819,14 +3157,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="2"/>
     </row>
   </sheetData>
@@ -3836,14 +3174,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="51.140625" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -3852,7 +3190,7 @@
     <col min="5" max="5" width="78.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="15" t="s">
         <v>230</v>
       </c>
@@ -3870,7 +3208,7 @@
       </c>
       <c r="H1" s="15"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="16" t="s">
         <v>234</v>
       </c>
@@ -3881,7 +3219,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="16" t="s">
         <v>235</v>
       </c>
@@ -3889,7 +3227,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="16" t="s">
         <v>236</v>
       </c>
@@ -3897,7 +3235,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="16" t="s">
         <v>237</v>
       </c>
@@ -3905,7 +3243,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" s="16" t="s">
         <v>238</v>
       </c>
@@ -3913,7 +3251,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="16" t="s">
         <v>239</v>
       </c>
@@ -3921,7 +3259,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="16" t="s">
         <v>240</v>
       </c>
@@ -3929,7 +3267,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="16" t="s">
         <v>241</v>
       </c>
@@ -3937,23 +3275,23 @@
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="25.5">
       <c r="A10" s="16" t="s">
         <v>242</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="21" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2">
       <c r="B17" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="D10" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -4496,14 +3834,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="6" width="2" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
@@ -4517,7 +3855,7 @@
     <col min="20" max="20" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:20">
       <c r="B2" s="5" t="s">
         <v>54</v>
       </c>
@@ -4560,13 +3898,13 @@
         <v>250</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:20" ht="38.25">
       <c r="B3" s="8" t="s">
         <v>69</v>
       </c>
@@ -4594,14 +3932,14 @@
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
     </row>
-    <row r="4" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:20" ht="25.5">
       <c r="B4" s="11"/>
       <c r="C4" s="12" t="s">
         <v>75</v>
@@ -4634,13 +3972,13 @@
         <v>251</v>
       </c>
       <c r="Q4" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:20" ht="38.25">
       <c r="B5" s="11"/>
       <c r="C5" s="12" t="s">
         <v>82</v>
@@ -4674,10 +4012,10 @@
         <v>89</v>
       </c>
       <c r="P5" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q5" s="19" t="s">
         <v>259</v>
-      </c>
-      <c r="Q5" s="19" t="s">
-        <v>260</v>
       </c>
       <c r="R5" s="19" t="s">
         <v>2</v>
@@ -4685,7 +4023,7 @@
       <c r="S5" s="19"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:20" ht="38.25">
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
         <v>90</v>
@@ -4719,10 +4057,10 @@
         <v>95</v>
       </c>
       <c r="P6" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Q6" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R6" s="19" t="s">
         <v>2</v>
@@ -4730,7 +4068,7 @@
       <c r="S6" s="19"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:20" ht="25.5">
       <c r="B7" s="11"/>
       <c r="C7" s="20" t="s">
         <v>96</v>
@@ -4762,10 +4100,10 @@
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="19" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="Q7" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R7" s="19" t="s">
         <v>2</v>
@@ -4773,7 +4111,7 @@
       <c r="S7" s="19"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:20" ht="38.25">
       <c r="B8" s="11"/>
       <c r="C8" s="20" t="s">
         <v>102</v>
@@ -4810,7 +4148,7 @@
         <v>256</v>
       </c>
       <c r="Q8" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R8" s="19" t="s">
         <v>2</v>
@@ -4818,7 +4156,7 @@
       <c r="S8" s="19"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:20" ht="38.25">
       <c r="B9" s="11"/>
       <c r="C9" s="20" t="s">
         <v>108</v>
@@ -4855,7 +4193,7 @@
         <v>255</v>
       </c>
       <c r="Q9" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R9" s="19" t="s">
         <v>2</v>
@@ -4863,7 +4201,7 @@
       <c r="S9" s="19"/>
       <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:20" ht="38.25">
       <c r="B10" s="11"/>
       <c r="C10" s="20" t="s">
         <v>114</v>
@@ -4900,7 +4238,7 @@
         <v>254</v>
       </c>
       <c r="Q10" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R10" s="19" t="s">
         <v>2</v>
@@ -4908,7 +4246,7 @@
       <c r="S10" s="19"/>
       <c r="T10" s="2"/>
     </row>
-    <row r="11" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:20" ht="38.25">
       <c r="B11" s="11"/>
       <c r="C11" s="20" t="s">
         <v>120</v>
@@ -4945,7 +4283,7 @@
         <v>253</v>
       </c>
       <c r="Q11" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R11" s="19" t="s">
         <v>2</v>
@@ -4953,7 +4291,7 @@
       <c r="S11" s="19"/>
       <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:20" ht="25.5">
       <c r="B12" s="11"/>
       <c r="C12" s="12" t="s">
         <v>126</v>
@@ -4988,7 +4326,7 @@
         <v>252</v>
       </c>
       <c r="Q12" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
@@ -4996,12 +4334,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O5" location="ToiletTrainednessUrineCodelist!A1" display="ToiletTrainednessUrineCodelist" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="O6" location="ToiletTrainednessFecesCodelist!A1" display="ToiletTrainednessFecesCodelist" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="O8" location="DevelopmentLocomotionCodelist!A1" display="DevelopmentLocomotionCodelist" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="O9" location="DevelopmentSocialCodelist!A1" display="DevelopmentSocialCodelist" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="O10" location="DevelopmentLinguisticsCodelist!A1" display="DevelopmentLinguisticsCodelist" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
-    <hyperlink ref="O11" location="DevelopmentCognitionCodelist!A1" display="DevelopmentCognitionCodelist" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="O5" location="ToiletTrainednessUrineCodelist!A1" display="ToiletTrainednessUrineCodelist"/>
+    <hyperlink ref="O6" location="ToiletTrainednessFecesCodelist!A1" display="ToiletTrainednessFecesCodelist"/>
+    <hyperlink ref="O8" location="DevelopmentLocomotionCodelist!A1" display="DevelopmentLocomotionCodelist"/>
+    <hyperlink ref="O9" location="DevelopmentSocialCodelist!A1" display="DevelopmentSocialCodelist"/>
+    <hyperlink ref="O10" location="DevelopmentLinguisticsCodelist!A1" display="DevelopmentLinguisticsCodelist"/>
+    <hyperlink ref="O11" location="DevelopmentCognitionCodelist!A1" display="DevelopmentCognitionCodelist"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -5012,12 +4350,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -5026,18 +4364,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="21" t="s">
+    <row r="3" spans="3:7">
+      <c r="C3" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="3:7">
       <c r="C4" s="14" t="s">
         <v>135</v>
       </c>
@@ -5054,7 +4392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:7">
       <c r="C5" s="2" t="s">
         <v>139</v>
       </c>
@@ -5071,7 +4409,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:7">
       <c r="C6" s="2" t="s">
         <v>144</v>
       </c>
@@ -5088,7 +4426,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:7" ht="25.5">
       <c r="C7" s="2" t="s">
         <v>147</v>
       </c>
@@ -5105,7 +4443,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:7" ht="25.5">
       <c r="C8" s="2" t="s">
         <v>150</v>
       </c>
@@ -5122,7 +4460,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:7" ht="25.5">
       <c r="C9" s="2" t="s">
         <v>153</v>
       </c>
@@ -5152,12 +4490,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -5166,18 +4504,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="21" t="s">
+    <row r="3" spans="3:7">
+      <c r="C3" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="3:7">
       <c r="C4" s="14" t="s">
         <v>135</v>
       </c>
@@ -5194,7 +4532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:7">
       <c r="C5" s="2" t="s">
         <v>157</v>
       </c>
@@ -5211,7 +4549,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:7" ht="25.5">
       <c r="C6" s="2" t="s">
         <v>160</v>
       </c>
@@ -5228,7 +4566,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:7" ht="25.5">
       <c r="C7" s="2" t="s">
         <v>163</v>
       </c>
@@ -5245,7 +4583,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:7" ht="25.5">
       <c r="C8" s="2" t="s">
         <v>166</v>
       </c>
@@ -5262,7 +4600,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:7" ht="25.5">
       <c r="C9" s="2" t="s">
         <v>169</v>
       </c>
@@ -5292,12 +4630,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -5306,18 +4644,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="21" t="s">
+    <row r="3" spans="3:7">
+      <c r="C3" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="3:7">
       <c r="C4" s="14" t="s">
         <v>135</v>
       </c>
@@ -5334,7 +4672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:7">
       <c r="C5" s="2" t="s">
         <v>173</v>
       </c>
@@ -5351,7 +4689,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:7">
       <c r="C6" s="2" t="s">
         <v>176</v>
       </c>
@@ -5368,7 +4706,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:7">
       <c r="C7" s="2" t="s">
         <v>179</v>
       </c>
@@ -5385,7 +4723,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:7" ht="25.5">
       <c r="C8" s="2" t="s">
         <v>182</v>
       </c>
@@ -5402,7 +4740,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:7">
       <c r="C9" s="2" t="s">
         <v>185</v>
       </c>
@@ -5432,12 +4770,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -5446,18 +4784,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="21" t="s">
+    <row r="3" spans="3:7">
+      <c r="C3" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="3:7">
       <c r="C4" s="14" t="s">
         <v>135</v>
       </c>
@@ -5474,7 +4812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:7" ht="25.5">
       <c r="C5" s="2" t="s">
         <v>189</v>
       </c>
@@ -5491,7 +4829,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:7" ht="25.5">
       <c r="C6" s="2" t="s">
         <v>192</v>
       </c>
@@ -5508,7 +4846,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:7" ht="25.5">
       <c r="C7" s="2" t="s">
         <v>195</v>
       </c>
@@ -5525,7 +4863,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:7" ht="25.5">
       <c r="C8" s="2" t="s">
         <v>198</v>
       </c>
@@ -5542,7 +4880,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:7" ht="25.5">
       <c r="C9" s="2" t="s">
         <v>201</v>
       </c>

</xml_diff>

<commit_message>
fix: recreated valuesets and profile for DevelopmentChild
</commit_message>
<xml_diff>
--- a/Mappings/DevelopmentChild - STU3.xlsx
+++ b/Mappings/DevelopmentChild - STU3.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edelman\Nictiz-STU3-Zib2017\Mappings\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26DF402-D565-4D88-BDA2-A128B35D08C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13995" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13995" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -807,9 +801,6 @@
     <t>.component.developmentLocomotion.valueCodeableConcept</t>
   </si>
   <si>
-    <t>.component.ageFirstMenstruation.valueCodeableConcept</t>
-  </si>
-  <si>
     <t>.component.toiletTrainednessFeces.valueCodeableConcept</t>
   </si>
   <si>
@@ -823,13 +814,16 @@
   </si>
   <si>
     <t>nl-core-observation</t>
+  </si>
+  <si>
+    <t>.component.ageFirstMenstruation.valueDateTime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -1022,11 +1016,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1157,7 +1151,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1198,7 +1192,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1239,7 +1233,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1294,14 +1288,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3073"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000010C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1309,29 +1300,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1361,14 +1329,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3074"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000020C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1376,29 +1341,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1428,14 +1370,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3075"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000030C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1443,29 +1382,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1495,14 +1411,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3076"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000040C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1510,29 +1423,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1562,14 +1452,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3077"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000050C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1577,29 +1464,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1629,14 +1493,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3078"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000060C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1644,29 +1505,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1696,14 +1534,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3079"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000070C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1711,29 +1546,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1763,14 +1575,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3080"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000080C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1778,29 +1587,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1830,14 +1616,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3081"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000090C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1845,29 +1628,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1897,14 +1657,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3082"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1912,29 +1669,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1964,14 +1698,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3083"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1979,29 +1710,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2031,14 +1739,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3084"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2046,29 +1751,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2098,14 +1780,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3085"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2113,29 +1792,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2165,14 +1821,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3086"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2180,29 +1833,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2232,14 +1862,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3087"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000F0C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2247,29 +1874,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2299,14 +1903,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3088"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000100C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2314,29 +1915,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2366,14 +1944,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3089"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000110C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2381,29 +1956,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2433,14 +1985,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3090"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000120C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2448,29 +1997,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2500,14 +2026,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3091"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000130C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2515,29 +2038,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2567,14 +2067,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3092"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000140C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2582,29 +2079,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2634,14 +2108,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3093"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000150C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2649,29 +2120,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2701,14 +2149,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3094"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000160C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2716,29 +2161,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2768,14 +2190,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3095"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000170C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2783,29 +2202,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2835,14 +2231,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s3096"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000180C0000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2850,29 +2243,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2926,7 +2296,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2959,26 +2329,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3011,23 +2364,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3203,18 +2539,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3222,7 +2558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -3230,7 +2566,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -3238,7 +2574,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -3246,7 +2582,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -3254,7 +2590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -3262,7 +2598,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -3270,7 +2606,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3">
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
@@ -3278,7 +2614,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3">
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
@@ -3286,7 +2622,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3">
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
@@ -3294,7 +2630,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3" ht="38.25">
       <c r="B12" s="2" t="s">
         <v>54</v>
       </c>
@@ -3302,7 +2638,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3" ht="63.75">
       <c r="B13" s="2" t="s">
         <v>56</v>
       </c>
@@ -3310,7 +2646,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3" ht="38.25">
       <c r="B14" s="2" t="s">
         <v>58</v>
       </c>
@@ -3318,7 +2654,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:3" ht="51">
       <c r="B15" s="2" t="s">
         <v>132</v>
       </c>
@@ -3328,7 +2664,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3339,12 +2675,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:G3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -3353,18 +2691,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="21" t="s">
+    <row r="3" spans="3:7">
+      <c r="C3" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="3:7">
       <c r="C4" s="14" t="s">
         <v>135</v>
       </c>
@@ -3381,7 +2719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:7" ht="25.5">
       <c r="C5" s="2" t="s">
         <v>205</v>
       </c>
@@ -3398,7 +2736,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:7" ht="25.5">
       <c r="C6" s="2" t="s">
         <v>208</v>
       </c>
@@ -3415,7 +2753,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:7" ht="25.5">
       <c r="C7" s="2" t="s">
         <v>211</v>
       </c>
@@ -3445,12 +2783,12 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -3459,18 +2797,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="21" t="s">
+    <row r="3" spans="3:7">
+      <c r="C3" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="3:7">
       <c r="C4" s="14" t="s">
         <v>135</v>
       </c>
@@ -3487,7 +2825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:7" ht="25.5">
       <c r="C5" s="2" t="s">
         <v>215</v>
       </c>
@@ -3504,7 +2842,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:7" ht="25.5">
       <c r="C6" s="2" t="s">
         <v>217</v>
       </c>
@@ -3521,7 +2859,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:7" ht="25.5">
       <c r="C7" s="2" t="s">
         <v>220</v>
       </c>
@@ -3538,7 +2876,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:7" ht="25.5">
       <c r="C8" s="2" t="s">
         <v>222</v>
       </c>
@@ -3568,42 +2906,42 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="150" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:2">
       <c r="B2" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:2" ht="140.25">
       <c r="B3" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:2">
       <c r="B4" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:2" ht="25.5">
       <c r="B5" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:2">
       <c r="B6" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:2" ht="38.25">
       <c r="B7" s="2" t="s">
         <v>229</v>
       </c>
@@ -3614,24 +2952,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="21" t="s">
+    <row r="2" spans="2:3">
+      <c r="B2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="21"/>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C2" s="22"/>
+    </row>
+    <row r="3" spans="2:3">
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
@@ -3639,7 +2977,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3">
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
@@ -3647,7 +2985,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3">
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
@@ -3655,7 +2993,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3">
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
@@ -3663,7 +3001,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -3671,7 +3009,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3">
       <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
@@ -3679,13 +3017,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3">
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3">
       <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
@@ -3693,25 +3031,25 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3">
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3">
       <c r="B13" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3">
       <c r="B14" s="2" t="s">
         <v>36</v>
       </c>
@@ -3719,7 +3057,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:3">
       <c r="B15" s="2" t="s">
         <v>38</v>
       </c>
@@ -3727,7 +3065,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:3">
       <c r="B16" s="2" t="s">
         <v>40</v>
       </c>
@@ -3735,7 +3073,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3">
       <c r="B17" s="2" t="s">
         <v>41</v>
       </c>
@@ -3743,7 +3081,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3">
       <c r="B18" s="2" t="s">
         <v>42</v>
       </c>
@@ -3751,7 +3089,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3">
       <c r="B19" s="2" t="s">
         <v>44</v>
       </c>
@@ -3759,7 +3097,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3">
       <c r="B20" s="2" t="s">
         <v>45</v>
       </c>
@@ -3767,7 +3105,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3">
       <c r="B21" s="2" t="s">
         <v>46</v>
       </c>
@@ -3775,7 +3113,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3">
       <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
@@ -3783,7 +3121,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3">
       <c r="B23" s="2" t="s">
         <v>49</v>
       </c>
@@ -3791,7 +3129,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3">
       <c r="B24" s="2" t="s">
         <v>51</v>
       </c>
@@ -3799,7 +3137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3">
       <c r="B25" s="2" t="s">
         <v>52</v>
       </c>
@@ -3819,14 +3157,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="2"/>
     </row>
   </sheetData>
@@ -3836,14 +3174,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="51.140625" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -3852,7 +3190,7 @@
     <col min="5" max="5" width="78.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="15" t="s">
         <v>230</v>
       </c>
@@ -3870,7 +3208,7 @@
       </c>
       <c r="H1" s="15"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="16" t="s">
         <v>234</v>
       </c>
@@ -3881,7 +3219,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="16" t="s">
         <v>235</v>
       </c>
@@ -3889,7 +3227,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="16" t="s">
         <v>236</v>
       </c>
@@ -3897,7 +3235,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="16" t="s">
         <v>237</v>
       </c>
@@ -3905,7 +3243,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" s="16" t="s">
         <v>238</v>
       </c>
@@ -3913,7 +3251,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="16" t="s">
         <v>239</v>
       </c>
@@ -3921,7 +3259,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="16" t="s">
         <v>240</v>
       </c>
@@ -3929,7 +3267,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="16" t="s">
         <v>241</v>
       </c>
@@ -3937,23 +3275,23 @@
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="25.5">
       <c r="A10" s="16" t="s">
         <v>242</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="21" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2">
       <c r="B17" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="D10" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -4496,14 +3834,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="6" width="2" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
@@ -4517,7 +3855,7 @@
     <col min="20" max="20" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:20">
       <c r="B2" s="5" t="s">
         <v>54</v>
       </c>
@@ -4560,13 +3898,13 @@
         <v>250</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:20" ht="38.25">
       <c r="B3" s="8" t="s">
         <v>69</v>
       </c>
@@ -4594,14 +3932,14 @@
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
     </row>
-    <row r="4" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:20" ht="25.5">
       <c r="B4" s="11"/>
       <c r="C4" s="12" t="s">
         <v>75</v>
@@ -4634,13 +3972,13 @@
         <v>251</v>
       </c>
       <c r="Q4" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:20" ht="38.25">
       <c r="B5" s="11"/>
       <c r="C5" s="12" t="s">
         <v>82</v>
@@ -4674,10 +4012,10 @@
         <v>89</v>
       </c>
       <c r="P5" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q5" s="19" t="s">
         <v>259</v>
-      </c>
-      <c r="Q5" s="19" t="s">
-        <v>260</v>
       </c>
       <c r="R5" s="19" t="s">
         <v>2</v>
@@ -4685,7 +4023,7 @@
       <c r="S5" s="19"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:20" ht="38.25">
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
         <v>90</v>
@@ -4719,10 +4057,10 @@
         <v>95</v>
       </c>
       <c r="P6" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Q6" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R6" s="19" t="s">
         <v>2</v>
@@ -4730,7 +4068,7 @@
       <c r="S6" s="19"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:20" ht="25.5">
       <c r="B7" s="11"/>
       <c r="C7" s="20" t="s">
         <v>96</v>
@@ -4762,10 +4100,10 @@
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="19" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="Q7" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R7" s="19" t="s">
         <v>2</v>
@@ -4773,7 +4111,7 @@
       <c r="S7" s="19"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:20" ht="38.25">
       <c r="B8" s="11"/>
       <c r="C8" s="20" t="s">
         <v>102</v>
@@ -4810,7 +4148,7 @@
         <v>256</v>
       </c>
       <c r="Q8" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R8" s="19" t="s">
         <v>2</v>
@@ -4818,7 +4156,7 @@
       <c r="S8" s="19"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:20" ht="38.25">
       <c r="B9" s="11"/>
       <c r="C9" s="20" t="s">
         <v>108</v>
@@ -4855,7 +4193,7 @@
         <v>255</v>
       </c>
       <c r="Q9" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R9" s="19" t="s">
         <v>2</v>
@@ -4863,7 +4201,7 @@
       <c r="S9" s="19"/>
       <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:20" ht="38.25">
       <c r="B10" s="11"/>
       <c r="C10" s="20" t="s">
         <v>114</v>
@@ -4900,7 +4238,7 @@
         <v>254</v>
       </c>
       <c r="Q10" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R10" s="19" t="s">
         <v>2</v>
@@ -4908,7 +4246,7 @@
       <c r="S10" s="19"/>
       <c r="T10" s="2"/>
     </row>
-    <row r="11" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:20" ht="38.25">
       <c r="B11" s="11"/>
       <c r="C11" s="20" t="s">
         <v>120</v>
@@ -4945,7 +4283,7 @@
         <v>253</v>
       </c>
       <c r="Q11" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R11" s="19" t="s">
         <v>2</v>
@@ -4953,7 +4291,7 @@
       <c r="S11" s="19"/>
       <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:20" ht="25.5">
       <c r="B12" s="11"/>
       <c r="C12" s="12" t="s">
         <v>126</v>
@@ -4988,7 +4326,7 @@
         <v>252</v>
       </c>
       <c r="Q12" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
@@ -4996,12 +4334,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O5" location="ToiletTrainednessUrineCodelist!A1" display="ToiletTrainednessUrineCodelist" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="O6" location="ToiletTrainednessFecesCodelist!A1" display="ToiletTrainednessFecesCodelist" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="O8" location="DevelopmentLocomotionCodelist!A1" display="DevelopmentLocomotionCodelist" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="O9" location="DevelopmentSocialCodelist!A1" display="DevelopmentSocialCodelist" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="O10" location="DevelopmentLinguisticsCodelist!A1" display="DevelopmentLinguisticsCodelist" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
-    <hyperlink ref="O11" location="DevelopmentCognitionCodelist!A1" display="DevelopmentCognitionCodelist" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="O5" location="ToiletTrainednessUrineCodelist!A1" display="ToiletTrainednessUrineCodelist"/>
+    <hyperlink ref="O6" location="ToiletTrainednessFecesCodelist!A1" display="ToiletTrainednessFecesCodelist"/>
+    <hyperlink ref="O8" location="DevelopmentLocomotionCodelist!A1" display="DevelopmentLocomotionCodelist"/>
+    <hyperlink ref="O9" location="DevelopmentSocialCodelist!A1" display="DevelopmentSocialCodelist"/>
+    <hyperlink ref="O10" location="DevelopmentLinguisticsCodelist!A1" display="DevelopmentLinguisticsCodelist"/>
+    <hyperlink ref="O11" location="DevelopmentCognitionCodelist!A1" display="DevelopmentCognitionCodelist"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -5012,12 +4350,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -5026,18 +4364,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="21" t="s">
+    <row r="3" spans="3:7">
+      <c r="C3" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="3:7">
       <c r="C4" s="14" t="s">
         <v>135</v>
       </c>
@@ -5054,7 +4392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:7">
       <c r="C5" s="2" t="s">
         <v>139</v>
       </c>
@@ -5071,7 +4409,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:7">
       <c r="C6" s="2" t="s">
         <v>144</v>
       </c>
@@ -5088,7 +4426,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:7" ht="25.5">
       <c r="C7" s="2" t="s">
         <v>147</v>
       </c>
@@ -5105,7 +4443,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:7" ht="25.5">
       <c r="C8" s="2" t="s">
         <v>150</v>
       </c>
@@ -5122,7 +4460,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:7" ht="25.5">
       <c r="C9" s="2" t="s">
         <v>153</v>
       </c>
@@ -5152,12 +4490,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -5166,18 +4504,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="21" t="s">
+    <row r="3" spans="3:7">
+      <c r="C3" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="3:7">
       <c r="C4" s="14" t="s">
         <v>135</v>
       </c>
@@ -5194,7 +4532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:7">
       <c r="C5" s="2" t="s">
         <v>157</v>
       </c>
@@ -5211,7 +4549,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:7" ht="25.5">
       <c r="C6" s="2" t="s">
         <v>160</v>
       </c>
@@ -5228,7 +4566,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:7" ht="25.5">
       <c r="C7" s="2" t="s">
         <v>163</v>
       </c>
@@ -5245,7 +4583,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:7" ht="25.5">
       <c r="C8" s="2" t="s">
         <v>166</v>
       </c>
@@ -5262,7 +4600,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:7" ht="25.5">
       <c r="C9" s="2" t="s">
         <v>169</v>
       </c>
@@ -5292,12 +4630,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -5306,18 +4644,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="21" t="s">
+    <row r="3" spans="3:7">
+      <c r="C3" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="3:7">
       <c r="C4" s="14" t="s">
         <v>135</v>
       </c>
@@ -5334,7 +4672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:7">
       <c r="C5" s="2" t="s">
         <v>173</v>
       </c>
@@ -5351,7 +4689,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:7">
       <c r="C6" s="2" t="s">
         <v>176</v>
       </c>
@@ -5368,7 +4706,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:7">
       <c r="C7" s="2" t="s">
         <v>179</v>
       </c>
@@ -5385,7 +4723,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:7" ht="25.5">
       <c r="C8" s="2" t="s">
         <v>182</v>
       </c>
@@ -5402,7 +4740,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:7">
       <c r="C9" s="2" t="s">
         <v>185</v>
       </c>
@@ -5432,12 +4770,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -5446,18 +4784,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="21" t="s">
+    <row r="3" spans="3:7">
+      <c r="C3" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="3:7">
       <c r="C4" s="14" t="s">
         <v>135</v>
       </c>
@@ -5474,7 +4812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:7" ht="25.5">
       <c r="C5" s="2" t="s">
         <v>189</v>
       </c>
@@ -5491,7 +4829,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:7" ht="25.5">
       <c r="C6" s="2" t="s">
         <v>192</v>
       </c>
@@ -5508,7 +4846,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:7" ht="25.5">
       <c r="C7" s="2" t="s">
         <v>195</v>
       </c>
@@ -5525,7 +4863,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:7" ht="25.5">
       <c r="C8" s="2" t="s">
         <v>198</v>
       </c>
@@ -5542,7 +4880,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:7" ht="25.5">
       <c r="C9" s="2" t="s">
         <v>201</v>
       </c>

</xml_diff>